<commit_message>
tried debugging display and v2 of pcb
</commit_message>
<xml_diff>
--- a/pcb/carl/Project Outputs for carl/Fabrication/BOM/PCB-00001-01_BOM-carl.xlsx
+++ b/pcb/carl/Project Outputs for carl/Fabrication/BOM/PCB-00001-01_BOM-carl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swift\AppData\Local\TempReleases\Snapshot\1\Fabrication\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EA183E7-5685-47C2-AABD-001146CE5827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEF03FF3-C3B6-48AE-A3F5-32A66743766C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5688" yWindow="2604" windowWidth="17280" windowHeight="9048" xr2:uid="{33A75755-761E-4A93-ADB5-4C397E40FC24}"/>
+    <workbookView xWindow="5688" yWindow="2604" windowWidth="17280" windowHeight="9048" xr2:uid="{7B656C43-30A1-4BD1-BCDF-4443AEEC1804}"/>
   </bookViews>
   <sheets>
     <sheet name="PCB-00001-01_BOM-carl" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
   <si>
     <t>Designator</t>
   </si>
@@ -107,6 +107,12 @@
     <t>CAP CER 0.1UF 50V X7R 0805</t>
   </si>
   <si>
+    <t>C7, C9</t>
+  </si>
+  <si>
+    <t>C8, C10</t>
+  </si>
+  <si>
     <t>D1, D2, D3, D4, D5, D6, D7, D8</t>
   </si>
   <si>
@@ -143,7 +149,7 @@
     <t>J4</t>
   </si>
   <si>
-    <t>J5</t>
+    <t>J5, J10</t>
   </si>
   <si>
     <t>Harwin</t>
@@ -264,6 +270,18 @@
   </si>
   <si>
     <t>RES Thick Film, 220Ω, 1%, 0.125W, 100ppm/°C, 0805</t>
+  </si>
+  <si>
+    <t>R37, R39</t>
+  </si>
+  <si>
+    <t>Vishay Semiconductor</t>
+  </si>
+  <si>
+    <t>Chip Resistor, 10 KOhm, +/- 1%, 100 mW, -55 to 155 degC, 0603 (1608 Metric), RoHS, Tape and Reel</t>
+  </si>
+  <si>
+    <t>R38, R40</t>
   </si>
   <si>
     <t>SW1</t>
@@ -681,8 +699,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{848845F7-BBE7-4FB7-9BCA-FDE089AB7C67}">
-  <dimension ref="A1:E38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6054AA09-1472-4080-A44F-87CE66DBC5D3}">
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -797,124 +815,124 @@
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1"/>
       <c r="D7" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -922,14 +940,14 @@
         <v>39</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -937,16 +955,14 @@
         <v>40</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -954,44 +970,46 @@
         <v>41</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="D18" s="1">
         <v>1</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1">
         <v>1</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -999,14 +1017,14 @@
         <v>46</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1">
         <v>1</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1014,14 +1032,14 @@
         <v>47</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1029,136 +1047,132 @@
         <v>48</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
         <v>1</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1">
         <v>1</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1">
         <v>1</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>56</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1">
         <v>1</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="1"/>
       <c r="D26" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="C27" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D27" s="1">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>64</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B28" s="1"/>
       <c r="C28" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D28" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="1">
+        <v>18</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
@@ -1169,16 +1183,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D31" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>15</v>
@@ -1186,103 +1200,167 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="C32" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D32" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="C33" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D33" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D34" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B35" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B36" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D37" s="1">
         <v>1</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D38" s="1">
-        <v>1</v>
-      </c>
-      <c r="E38" s="2" t="s">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="2" t="s">
         <v>88</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>